<commit_message>
all data + code put into report, some minor text left
</commit_message>
<xml_diff>
--- a/Assignment1/Book1.xlsx
+++ b/Assignment1/Book1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t>N</t>
   </si>
@@ -64,10 +64,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -145,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -159,6 +166,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -291,11 +301,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="104573568"/>
-        <c:axId val="104592128"/>
+        <c:axId val="89500288"/>
+        <c:axId val="89518848"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="104573568"/>
+        <c:axId val="89500288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -320,12 +330,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104592128"/>
+        <c:crossAx val="89518848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="104592128"/>
+        <c:axId val="89518848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -352,7 +362,7 @@
         </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104573568"/>
+        <c:crossAx val="89500288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -361,7 +371,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -489,11 +499,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="105010304"/>
-        <c:axId val="105012224"/>
+        <c:axId val="89547904"/>
+        <c:axId val="89549824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="105010304"/>
+        <c:axId val="89547904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -518,12 +528,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105012224"/>
+        <c:crossAx val="89549824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="105012224"/>
+        <c:axId val="89549824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -550,7 +560,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="105010304"/>
+        <c:crossAx val="89547904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -559,7 +569,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -688,11 +698,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="106039936"/>
-        <c:axId val="106050304"/>
+        <c:axId val="89586304"/>
+        <c:axId val="96346880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106039936"/>
+        <c:axId val="89586304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,12 +727,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106050304"/>
+        <c:crossAx val="96346880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106050304"/>
+        <c:axId val="96346880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -748,7 +758,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106039936"/>
+        <c:crossAx val="89586304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -757,7 +767,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -821,7 +831,7 @@
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-5.8709973753280839E-2"/>
-                  <c:y val="-5.6499708369787099E-2"/>
+                  <c:y val="-5.6499708369787092E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -846,10 +856,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$78:$A$86</c:f>
+              <c:f>Sheet1!$A$78:$A$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -876,16 +886,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$78:$C$86</c:f>
+              <c:f>Sheet1!$C$78:$C$88</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="11"/>
                 <c:pt idx="0">
                   <c:v>1.1111298767100153</c:v>
                 </c:pt>
@@ -912,16 +928,22 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>2.5443396895158439</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.8102495713469238</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.9575747981636851</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="106079360"/>
-        <c:axId val="106081280"/>
+        <c:axId val="96380032"/>
+        <c:axId val="96381952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="106079360"/>
+        <c:axId val="96380032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -946,12 +968,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106081280"/>
+        <c:crossAx val="96381952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="106081280"/>
+        <c:axId val="96381952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -977,7 +999,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="106079360"/>
+        <c:crossAx val="96380032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -986,7 +1008,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1117,11 +1139,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="52678656"/>
-        <c:axId val="52676864"/>
+        <c:axId val="92088960"/>
+        <c:axId val="92095232"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52678656"/>
+        <c:axId val="92088960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="1"/>
@@ -1147,12 +1169,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52676864"/>
+        <c:crossAx val="92095232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="52676864"/>
+        <c:axId val="92095232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,7 +1200,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52678656"/>
+        <c:crossAx val="92088960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1187,7 +1209,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1283,11 +1305,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="73409664"/>
-        <c:axId val="73407872"/>
+        <c:axId val="96371072"/>
+        <c:axId val="96372992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="73409664"/>
+        <c:axId val="96371072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1312,12 +1334,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73407872"/>
+        <c:crossAx val="96372992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="73407872"/>
+        <c:axId val="96372992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1343,7 +1365,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="73409664"/>
+        <c:crossAx val="96371072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1352,7 +1374,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1456,11 +1478,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="116752384"/>
-        <c:axId val="116737536"/>
+        <c:axId val="96417664"/>
+        <c:axId val="96440320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="116752384"/>
+        <c:axId val="96417664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,12 +1507,12 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116737536"/>
+        <c:crossAx val="96440320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="116737536"/>
+        <c:axId val="96440320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1521,7 +1543,342 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116752384"/>
+        <c:crossAx val="96417664"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-CA"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Iterations vs 1/h [Jacobi]</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$142</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Number of iterations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$143:$B$147</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$143:$C$147</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>279</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>991</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3422</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11485</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="98027008"/>
+        <c:axId val="98025472"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="98027008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>1/h</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98025472"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="98025472"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Number of Iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="98027008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-CA"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>(0.06,0.04) potential</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> vs 1/h [Jacobi]</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$142</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>(0.06,0.04) potential (V)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$143:$B$147</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>800</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$143:$D$147</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.6842175217599999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.56707335729</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5260199946799999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5099085626200002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5012468712099998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:axId val="111066496"/>
+        <c:axId val="111063808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="111066496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>1/h</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="111063808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="111063808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-CA"/>
+                  <a:t>Point Potential (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="111066496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1743,6 +2100,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>138</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>156</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>170</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2036,16 +2453,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D116"/>
+  <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="N124" sqref="N124"/>
+    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+      <selection activeCell="D149" sqref="D149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -2452,7 +2870,7 @@
         <v>0.58823999999999999</v>
       </c>
       <c r="C79">
-        <f t="shared" ref="C79:C86" si="2">B79/(1-B79)</f>
+        <f t="shared" ref="C79:C88" si="2">B79/(1-B79)</f>
         <v>1.428599183990674</v>
       </c>
     </row>
@@ -2540,8 +2958,32 @@
         <v>2.5443396895158439</v>
       </c>
     </row>
+    <row r="87" spans="1:3">
+      <c r="A87">
+        <v>13</v>
+      </c>
+      <c r="B87">
+        <v>0.73755000000000004</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="2"/>
+        <v>2.8102495713469238</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88">
+        <v>15</v>
+      </c>
+      <c r="B88">
+        <v>0.74731999999999998</v>
+      </c>
+      <c r="C88">
+        <f t="shared" si="2"/>
+        <v>2.9575747981636851</v>
+      </c>
+    </row>
     <row r="93" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="94" spans="1:3" ht="60.75" thickBot="1">
+    <row r="94" spans="1:3" ht="15.75" thickBot="1">
       <c r="A94" s="2" t="s">
         <v>8</v>
       </c>
@@ -2750,6 +3192,91 @@
       </c>
       <c r="D116" s="5">
         <v>3.5009872104299999</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="15.75" thickBot="1"/>
+    <row r="142" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A142" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A143" s="4">
+        <v>0.02</v>
+      </c>
+      <c r="B143" s="6">
+        <v>50</v>
+      </c>
+      <c r="C143" s="5">
+        <v>75</v>
+      </c>
+      <c r="D143" s="5">
+        <v>3.6842175217599999</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A144" s="4">
+        <v>0.01</v>
+      </c>
+      <c r="B144" s="6">
+        <v>100</v>
+      </c>
+      <c r="C144" s="5">
+        <v>279</v>
+      </c>
+      <c r="D144" s="5">
+        <v>3.56707335729</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A145" s="4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B145" s="6">
+        <v>200</v>
+      </c>
+      <c r="C145" s="5">
+        <v>991</v>
+      </c>
+      <c r="D145" s="5">
+        <v>3.5260199946799999</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A146" s="4">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="B146" s="6">
+        <v>400</v>
+      </c>
+      <c r="C146" s="5">
+        <v>3422</v>
+      </c>
+      <c r="D146" s="5">
+        <v>3.5099085626200002</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A147" s="4">
+        <v>1.25E-3</v>
+      </c>
+      <c r="B147" s="6">
+        <v>800</v>
+      </c>
+      <c r="C147" s="5">
+        <v>11485</v>
+      </c>
+      <c r="D147" s="5">
+        <v>3.5012468712099998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>